<commit_message>
now got working asserts
</commit_message>
<xml_diff>
--- a/src/main/resources/TestWorksheet.xlsx
+++ b/src/main/resources/TestWorksheet.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="15">
   <si>
     <t>Input #</t>
   </si>
@@ -36,9 +36,6 @@
     <t>http://www.autotrader.co.uk/</t>
   </si>
   <si>
-    <t>NG15 6TF</t>
-  </si>
-  <si>
     <t xml:space="preserve">Within 30 miles </t>
   </si>
   <si>
@@ -48,9 +45,6 @@
     <t>value Car</t>
   </si>
   <si>
-    <t>HD54 LTF</t>
-  </si>
-  <si>
     <t>shreya.gund@qa.com</t>
   </si>
   <si>
@@ -58,6 +52,15 @@
   </si>
   <si>
     <t>Sign in</t>
+  </si>
+  <si>
+    <t>Redirecting to Plant</t>
+  </si>
+  <si>
+    <t>NG156TF</t>
+  </si>
+  <si>
+    <t>HD54LTF</t>
   </si>
 </sst>
 </file>
@@ -410,7 +413,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -444,16 +447,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
       </c>
       <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" t="s">
         <v>6</v>
-      </c>
-      <c r="E2" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -461,13 +464,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
         <v>5</v>
       </c>
       <c r="D3" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="E3">
         <v>50</v>
@@ -478,21 +481,24 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s">
         <v>5</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
       </c>
       <c r="C5" t="s">
         <v>5</v>

</xml_diff>